<commit_message>
Fix year of FMiA book chapter
</commit_message>
<xml_diff>
--- a/private/ADA_web_organizer.xlsx
+++ b/private/ADA_web_organizer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iicpe\Desktop\algorithmicdesign.github.io\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B28B8B-CE33-4A0B-8E84-EA46E12DE0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69465524-9E1D-45C0-8D68-BF792BCB9C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="525">
   <si>
     <t>GRAMATICA: A general 3D shape grammar interpreter targeting the mass customization of housing</t>
   </si>
@@ -1493,9 +1493,6 @@
     <t>Getting a handle on floor plan analysis: Door classification in floor plans and a survey on existing datasets</t>
   </si>
   <si>
-    <t>Behind Algorithmic Geometric Patterns: A framework for façade design exploration</t>
-  </si>
-  <si>
     <t>Converting algorithms into tangible solutions: a workflow for materializing algorithmic façade designs</t>
   </si>
   <si>
@@ -1625,7 +1622,7 @@
     <t>Behind Algorithmic Geometric Patterns: A Framework for Facade Design Exploration</t>
   </si>
   <si>
-    <t>Formal Methods in Architecture</t>
+    <t>actualizar o ano (de 22 para 23)</t>
   </si>
 </sst>
 </file>
@@ -2325,8 +2322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L313"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H104" sqref="H104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2389,7 +2386,7 @@
         <v>384</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>106</v>
@@ -2425,7 +2422,7 @@
         <v>383</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>35</v>
@@ -2437,7 +2434,7 @@
         <v>449</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -2515,18 +2512,18 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="G13" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="37" t="s">
+        <v>513</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>514</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>515</v>
       </c>
       <c r="D14" s="52" t="s">
         <v>291</v>
@@ -2553,10 +2550,10 @@
         <v>380</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D16" s="52" t="s">
         <v>291</v>
@@ -2569,10 +2566,10 @@
     <row r="17" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="57"/>
       <c r="B17" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D17" s="26">
         <v>2024</v>
@@ -2585,10 +2582,10 @@
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="57"/>
       <c r="B18" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D18" s="26">
         <v>2024</v>
@@ -2601,10 +2598,10 @@
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="57"/>
       <c r="B19" s="50" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D19" s="52" t="s">
         <v>291</v>
@@ -2620,10 +2617,10 @@
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="57"/>
       <c r="B20" s="50" t="s">
+        <v>502</v>
+      </c>
+      <c r="C20" s="51" t="s">
         <v>503</v>
-      </c>
-      <c r="C20" s="51" t="s">
-        <v>504</v>
       </c>
       <c r="D20" s="52" t="s">
         <v>291</v>
@@ -3568,25 +3565,25 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B68" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>144</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F68" s="22"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B69" s="54" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C69" s="54" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D69" s="54"/>
     </row>
@@ -3602,10 +3599,10 @@
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="3"/>
       <c r="B71" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>493</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>305</v>
@@ -3632,7 +3629,7 @@
         <v>479</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>378</v>
@@ -3641,13 +3638,13 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="3"/>
       <c r="B74" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>473</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>378</v>
@@ -3944,7 +3941,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
     </row>
-    <row r="97" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="B97" s="17" t="s">
         <v>355</v>
@@ -3962,13 +3959,13 @@
         <v>360</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="3"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" s="11">
         <v>2023</v>
       </c>
@@ -3977,22 +3974,25 @@
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B100" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>144</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>525</v>
+        <v>483</v>
       </c>
       <c r="F100" s="22"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G100" s="1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" s="3"/>
       <c r="B101" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>308</v>
@@ -4004,7 +4004,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" s="11">
         <v>2022</v>
       </c>
@@ -4013,37 +4013,29 @@
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="3"/>
-      <c r="B103" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="F103" s="33" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="F103" s="33"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="3"/>
       <c r="B104" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>144</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F104" s="33" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="11">
         <v>2021</v>
       </c>
@@ -4052,7 +4044,7 @@
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" s="3"/>
       <c r="B106" s="1" t="s">
         <v>365</v>
@@ -4068,7 +4060,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" s="3"/>
       <c r="B107" s="1" t="s">
         <v>354</v>
@@ -4084,7 +4076,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" s="3"/>
       <c r="B108" s="1" t="s">
         <v>348</v>
@@ -4093,14 +4085,14 @@
         <v>144</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E108" s="28"/>
       <c r="F108" s="33" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="11">
         <v>2015</v>
       </c>
@@ -4112,7 +4104,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B110" s="20" t="s">
         <v>47</v>
       </c>
@@ -4125,12 +4117,12 @@
       <c r="E110" s="28"/>
       <c r="F110" s="33"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
     </row>
-    <row r="112" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="2"/>
       <c r="B112" s="17" t="s">
         <v>258</v>
@@ -4172,7 +4164,7 @@
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" s="3"/>
       <c r="B116" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>366</v>
@@ -5511,13 +5503,13 @@
         <v>2023</v>
       </c>
       <c r="B213" s="7" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D213" s="7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.35">
@@ -5525,13 +5517,13 @@
         <v>2023</v>
       </c>
       <c r="B214" s="7" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>100</v>
       </c>
       <c r="D214" s="7" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.35">
@@ -5545,7 +5537,7 @@
         <v>81</v>
       </c>
       <c r="D215" s="7" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.35">
@@ -5707,7 +5699,7 @@
         <v>81</v>
       </c>
       <c r="B230" s="7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E230" s="6" t="s">
         <v>115</v>
@@ -5765,7 +5757,7 @@
         <v>35</v>
       </c>
       <c r="B237" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E237" s="6" t="s">
         <v>113</v>
@@ -5776,7 +5768,7 @@
         <v>106</v>
       </c>
       <c r="B238" s="7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E238" s="6" t="s">
         <v>244</v>
@@ -5787,7 +5779,7 @@
         <v>328</v>
       </c>
       <c r="B239" s="7" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E239" s="6" t="s">
         <v>112</v>
@@ -6489,10 +6481,10 @@
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="B303" s="7" t="s">
         <v>500</v>
-      </c>
-      <c r="B303" s="7" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add Renata's PhD Thesis
</commit_message>
<xml_diff>
--- a/private/ADA_web_organizer.xlsx
+++ b/private/ADA_web_organizer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iicpe\Desktop\algorithmicdesign.github.io\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69465524-9E1D-45C0-8D68-BF792BCB9C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCCC2C6-3B0D-406E-BBB1-FC7D6F8D17F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADA website control" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="525">
   <si>
     <t>GRAMATICA: A general 3D shape grammar interpreter targeting the mass customization of housing</t>
   </si>
@@ -1907,7 +1907,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2026,7 +2026,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2322,8 +2321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L313"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H104" sqref="H104"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2409,13 +2408,15 @@
         <v>328</v>
       </c>
       <c r="D5" s="26">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="22" t="s">
         <v>391</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" s="12" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="38" t="s">
@@ -4156,10 +4157,9 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" s="3"/>
-      <c r="B115" s="58"/>
-      <c r="C115" s="58"/>
-      <c r="D115" s="58"/>
-      <c r="E115" s="58"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" s="3"/>
@@ -5694,7 +5694,7 @@
       <c r="C229" s="10"/>
       <c r="D229" s="6"/>
     </row>
-    <row r="230" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A230" s="5" t="s">
         <v>81</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="237" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A237" s="5" t="s">
         <v>35</v>
       </c>

</xml_diff>